<commit_message>
Add settings, TDDied the organizations list, use FSharp data for parsing
</commit_message>
<xml_diff>
--- a/OperatorPortal/Tests/OrganizationsFromExcel/db_sample.xlsx
+++ b/OperatorPortal/Tests/OrganizationsFromExcel/db_sample.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="204">
   <si>
     <t xml:space="preserve">teczka</t>
   </si>
@@ -644,9 +644,6 @@
     <t xml:space="preserve">Samochody użyczone przez Fundację Ciepły Posiłek Renault Traffic 2 palety, Renault Master 8 palet</t>
   </si>
   <si>
-    <t xml:space="preserve">zaprzyjaźniony</t>
-  </si>
-  <si>
     <t xml:space="preserve">360409948</t>
   </si>
   <si>
@@ -784,6 +781,27 @@
   </si>
   <si>
     <t xml:space="preserve">fax.22  827 58 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dane adresowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dane adresowe ksiegowosci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontakty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Źródła żywności</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warunki udzielania pomocy żywnościowej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokumentacja</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1307,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1373,11 +1391,11 @@
   </sheetPr>
   <dimension ref="A1:AU13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP7" activeCellId="0" sqref="AP7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="35.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="35.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.54"/>
@@ -1397,9 +1415,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="10.9"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="20" style="2" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="21" min="21" style="0" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="18.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.54"/>
@@ -1409,13 +1427,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="32" style="0" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="36" style="0" width="3.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="2.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="3.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="3.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="4" width="10.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="7.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="7.64"/>
@@ -2371,8 +2389,9 @@
       <c r="AO7" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="AP7" s="33" t="s">
-        <v>151</v>
+      <c r="AP7" s="33" t="str">
+        <f aca="false">+P1</f>
+        <v> Tel. organ prowadzącego księgowość</v>
       </c>
       <c r="AQ7" s="56" t="n">
         <v>45436</v>
@@ -2401,10 +2420,10 @@
         <v>5311691463</v>
       </c>
       <c r="D8" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>152</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>153</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>74</v>
@@ -2413,22 +2432,22 @@
         <v>50</v>
       </c>
       <c r="H8" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="J8" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="K8" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="L8" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="M8" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>159</v>
       </c>
       <c r="N8" s="22" t="str">
         <f aca="false">H8</f>
@@ -2442,7 +2461,7 @@
         <v>987654321</v>
       </c>
       <c r="Q8" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R8" s="25" t="n">
         <v>123456789</v>
@@ -2454,7 +2473,7 @@
         <v>58</v>
       </c>
       <c r="W8" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X8" s="26" t="s">
         <v>60</v>
@@ -2473,7 +2492,7 @@
         <v>80</v>
       </c>
       <c r="AD8" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AE8" s="43"/>
       <c r="AF8" s="43"/>
@@ -2485,7 +2504,7 @@
         <v>63</v>
       </c>
       <c r="AJ8" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AK8" s="31"/>
       <c r="AL8" s="31"/>
@@ -2512,10 +2531,10 @@
         <v>9522107635</v>
       </c>
       <c r="D9" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="37" t="s">
         <v>164</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>165</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>74</v>
@@ -2524,16 +2543,16 @@
         <v>50</v>
       </c>
       <c r="H9" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J9" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="K9" s="21" t="s">
         <v>168</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>169</v>
       </c>
       <c r="L9" s="21" t="s">
         <v>53</v>
@@ -2542,16 +2561,16 @@
         <v>54</v>
       </c>
       <c r="N9" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P9" s="23" t="n">
         <v>987654321</v>
       </c>
       <c r="Q9" s="38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R9" s="25" t="n">
         <v>123456789</v>
@@ -2581,7 +2600,7 @@
         <v>33</v>
       </c>
       <c r="AD9" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AE9" s="43" t="s">
         <v>84</v>
@@ -2595,17 +2614,17 @@
         <v>63</v>
       </c>
       <c r="AJ9" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AK9" s="31"/>
       <c r="AL9" s="31"/>
       <c r="AM9" s="31"/>
       <c r="AN9" s="31"/>
       <c r="AO9" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP9" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="AP9" s="33" t="s">
-        <v>175</v>
       </c>
       <c r="AQ9" s="44"/>
       <c r="AR9" s="44"/>
@@ -2626,46 +2645,46 @@
         <v>9522107635</v>
       </c>
       <c r="D10" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>165</v>
-      </c>
       <c r="F10" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G10" s="60" t="s">
         <v>50</v>
       </c>
       <c r="H10" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>167</v>
-      </c>
       <c r="J10" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="K10" s="47" t="s">
+      <c r="L10" s="47" t="s">
         <v>178</v>
-      </c>
-      <c r="L10" s="47" t="s">
-        <v>179</v>
       </c>
       <c r="M10" s="47" t="s">
         <v>54</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P10" s="23" t="n">
         <v>987654321</v>
       </c>
       <c r="Q10" s="38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R10" s="25" t="n">
         <v>123456789</v>
@@ -2694,7 +2713,7 @@
         <v>18</v>
       </c>
       <c r="AD10" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AE10" s="43" t="s">
         <v>84</v>
@@ -2706,7 +2725,7 @@
         <v>63</v>
       </c>
       <c r="AJ10" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AK10" s="31"/>
       <c r="AL10" s="31"/>
@@ -2733,46 +2752,46 @@
         <v>5252265692</v>
       </c>
       <c r="D11" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="F11" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>182</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>50</v>
       </c>
       <c r="H11" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="J11" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="K11" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="L11" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>187</v>
       </c>
       <c r="M11" s="18" t="s">
         <v>54</v>
       </c>
       <c r="N11" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" s="46" t="s">
         <v>183</v>
-      </c>
-      <c r="O11" s="46" t="s">
-        <v>184</v>
       </c>
       <c r="P11" s="23" t="n">
         <v>987654321</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R11" s="25" t="n">
         <v>123456789</v>
@@ -2801,7 +2820,7 @@
         <v>40</v>
       </c>
       <c r="AD11" s="42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AE11" s="43"/>
       <c r="AF11" s="43"/>
@@ -2811,7 +2830,7 @@
         <v>63</v>
       </c>
       <c r="AJ11" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AK11" s="31"/>
       <c r="AL11" s="31"/>
@@ -2838,46 +2857,46 @@
         <v>5252265692</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>182</v>
       </c>
       <c r="G12" s="64" t="s">
         <v>50</v>
       </c>
       <c r="H12" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>184</v>
-      </c>
       <c r="J12" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="L12" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>195</v>
-      </c>
       <c r="N12" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="O12" s="46" t="s">
         <v>183</v>
-      </c>
-      <c r="O12" s="46" t="s">
-        <v>184</v>
       </c>
       <c r="P12" s="23" t="n">
         <v>987654321</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R12" s="25" t="n">
         <v>123456789</v>
@@ -2889,7 +2908,7 @@
         <v>601335206</v>
       </c>
       <c r="U12" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="V12" s="26" t="s">
         <v>58</v>
@@ -2910,7 +2929,7 @@
         <v>140</v>
       </c>
       <c r="AD12" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AE12" s="66"/>
       <c r="AF12" s="66"/>
@@ -2920,7 +2939,7 @@
         <v>63</v>
       </c>
       <c r="AJ12" s="67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AK12" s="67"/>
       <c r="AL12" s="67"/>
@@ -2935,9 +2954,29 @@
       <c r="AU12" s="68"/>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AC13" s="69" t="n">
-        <f aca="false">SUM(AC2:AC12)</f>
-        <v>2435</v>
+      <c r="B13" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC13" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ13" s="0" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>